<commit_message>
Delete the Delete Graphs Endpoint
</commit_message>
<xml_diff>
--- a/DATABASE/Bitácora.xlsx
+++ b/DATABASE/Bitácora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Documents\Escuela\6to Sem\Desarrollo de Software\Repositorios\TC3005B-E1\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F6FB74-227E-41AC-96C0-A4CDB3CBECA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E16A107-4237-48A6-BDE7-44F108F0BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AAF969ED-661E-4501-97C9-3B4CFFD775BB}"/>
   </bookViews>
@@ -264,10 +264,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -387,44 +387,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{217C3642-1A5E-4EB4-A8E7-58B1078FB4DB}" name="Table14" displayName="Table14" ref="A2:L18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{217C3642-1A5E-4EB4-A8E7-58B1078FB4DB}" name="Table14" displayName="Table14" ref="A2:L18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:L18" xr:uid="{217C3642-1A5E-4EB4-A8E7-58B1078FB4DB}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9C2B2D3E-011D-448A-BCFE-5B00CDE9A91D}" name="Sec" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{2FA85757-1016-4C3F-8450-4C7842A36923}" name="ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{108AB9A3-5080-453A-866C-B16A6B4E774F}" name="Descripción" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{8A2BC626-F3EA-4BF0-BFA7-41FD73891B04}" name="Caso / Precondición" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{A808F7FE-B028-42FB-B6A3-993108A3BA28}" name="Tipo" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{720907D5-1BDB-464E-8F1D-FB9B853D6E93}" name="Entrada Esperada" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{580F8D4A-8CC1-4136-940F-2B0C287196B5}" name="Entrada Dada" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2332772E-C521-42F7-A6EC-A69DB30DF8A3}" name="Salida Esperada" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{9C2B2D3E-011D-448A-BCFE-5B00CDE9A91D}" name="Sec" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{2FA85757-1016-4C3F-8450-4C7842A36923}" name="ID" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{108AB9A3-5080-453A-866C-B16A6B4E774F}" name="Descripción" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{8A2BC626-F3EA-4BF0-BFA7-41FD73891B04}" name="Caso / Precondición" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{A808F7FE-B028-42FB-B6A3-993108A3BA28}" name="Tipo" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{720907D5-1BDB-464E-8F1D-FB9B853D6E93}" name="Entrada Esperada" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{580F8D4A-8CC1-4136-940F-2B0C287196B5}" name="Entrada Dada" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{2332772E-C521-42F7-A6EC-A69DB30DF8A3}" name="Salida Esperada" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B7AEF90C-6BB4-4C94-B1A8-390E0BD4869A}" name="Salida Dada" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{CE7ADB74-9B9C-47FC-AB0D-63F98E5BAD64}" name="Tiempo" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{107D6FA5-4F86-423B-90FF-D0E45FD82F3F}" name="Comentarios" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{E0FFB7D1-4E10-4C28-93D6-06D233AA3F94}" name="Estatus" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{B7AEF90C-6BB4-4C94-B1A8-390E0BD4869A}" name="Salida Dada" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{CE7ADB74-9B9C-47FC-AB0D-63F98E5BAD64}" name="Tiempo" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{107D6FA5-4F86-423B-90FF-D0E45FD82F3F}" name="Comentarios" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{E0FFB7D1-4E10-4C28-93D6-06D233AA3F94}" name="Estatus" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:L18" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -730,7 +730,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32FBE0-3956-45F0-9B00-3537E8F21FB5}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -797,21 +799,21 @@
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1328,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5D3A1B-8CC9-40CC-BB08-44B34DB7A726}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1349,20 +1351,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Delete Documentation of Delete Graph
</commit_message>
<xml_diff>
--- a/DATABASE/Bitácora.xlsx
+++ b/DATABASE/Bitácora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Documents\Escuela\6to Sem\Desarrollo de Software\Repositorios\TC3005B-E1\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E16A107-4237-48A6-BDE7-44F108F0BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD149DF0-5AF6-40F8-A9C6-57FBAB1EFAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AAF969ED-661E-4501-97C9-3B4CFFD775BB}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AAF969ED-661E-4501-97C9-3B4CFFD775BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitácora" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -156,21 +156,9 @@
     <t>Caso / Precondición</t>
   </si>
   <si>
-    <t>BE-DG-C</t>
-  </si>
-  <si>
     <t>BE-PG-C</t>
   </si>
   <si>
-    <t>Borrar una gráfica por ID</t>
-  </si>
-  <si>
-    <t>BE-DG-I1</t>
-  </si>
-  <si>
-    <t>BE-DG-I2</t>
-  </si>
-  <si>
     <t>El graphID no existe</t>
   </si>
   <si>
@@ -198,28 +186,22 @@
     <t>ID_Template</t>
   </si>
   <si>
-    <t>TM-BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>BE-PG-I2-E</t>
   </si>
   <si>
     <t>BE-PG-I1-E</t>
   </si>
   <si>
-    <t>BE-DG-I1-E</t>
-  </si>
-  <si>
-    <t>BE-DG-C-E</t>
-  </si>
-  <si>
-    <t>BE-DG-I2-E</t>
-  </si>
-  <si>
     <t>BE-PG-C-E</t>
+  </si>
+  <si>
+    <t>BE-1</t>
+  </si>
+  <si>
+    <t>TM-BE-1</t>
+  </si>
+  <si>
+    <t>27/05/22</t>
   </si>
 </sst>
 </file>
@@ -387,44 +369,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{217C3642-1A5E-4EB4-A8E7-58B1078FB4DB}" name="Table14" displayName="Table14" ref="A2:L18" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A2:L18" xr:uid="{217C3642-1A5E-4EB4-A8E7-58B1078FB4DB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}" name="Table13" displayName="Table13" ref="A2:L15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A2:L15" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{9C2B2D3E-011D-448A-BCFE-5B00CDE9A91D}" name="Sec" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{2FA85757-1016-4C3F-8450-4C7842A36923}" name="ID" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{108AB9A3-5080-453A-866C-B16A6B4E774F}" name="Descripción" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{8A2BC626-F3EA-4BF0-BFA7-41FD73891B04}" name="Caso / Precondición" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{A808F7FE-B028-42FB-B6A3-993108A3BA28}" name="Tipo" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{720907D5-1BDB-464E-8F1D-FB9B853D6E93}" name="Entrada Esperada" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{580F8D4A-8CC1-4136-940F-2B0C287196B5}" name="Entrada Dada" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{2332772E-C521-42F7-A6EC-A69DB30DF8A3}" name="Salida Esperada" dataDxfId="18">
-      <calculatedColumnFormula>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{7B09FA86-D36E-427E-97CF-B7D8B36AB84D}" name="Sec" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{39FB757B-3C82-4EE3-B429-5F23FAE004D8}" name="ID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E942E4FC-8D92-4234-B6B1-D6F263244207}" name="Descripción" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{D732C358-F448-4B04-BBD0-ECFC5897E549}" name="Caso / Precondición" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{88CFCC99-ADBC-4B05-BF00-0D841EBA5F1A}" name="Tipo" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{BAB65155-53CC-4710-9605-1A048D68DF00}" name="Entrada Esperada" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{241B06ED-06A5-4504-9EC6-16FA523F3ED5}" name="Entrada Dada" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{2187D5F3-18A4-48C5-9F3F-BAA1BFEE46C7}" name="Salida Esperada" dataDxfId="4">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B7AEF90C-6BB4-4C94-B1A8-390E0BD4869A}" name="Salida Dada" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{CE7ADB74-9B9C-47FC-AB0D-63F98E5BAD64}" name="Tiempo" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{107D6FA5-4F86-423B-90FF-D0E45FD82F3F}" name="Comentarios" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{E0FFB7D1-4E10-4C28-93D6-06D233AA3F94}" name="Estatus" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{5C7873B5-E430-4D40-B78D-AE61CA6C7E13}" name="Salida Dada" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{0A23A4F0-5E33-44D3-9E82-A08C36D88BB2}" name="Tiempo" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{D8C2EF58-1D1F-4BD9-8949-5D5B023DF187}" name="Comentarios" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{2601F79F-09FF-427D-844A-A77E3E54B807}" name="Estatus" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A2:L18" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:L15" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -727,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32710F9C-3D4D-4EFE-8BF9-3040E30C63EB}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -745,22 +727,984 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A2+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A3+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A4+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A5+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A6+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A7+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A8+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A9+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A10+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A11+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A12+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A13+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A14+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A15+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A16+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A17+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A18+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A19+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A20+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A21+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A22+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A23+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A24+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A25+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A26+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A27+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A28+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A29+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A30+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A31+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A32+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A33+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A34+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A35+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A36+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A37+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A38+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A39+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A40+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A41+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A42+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A43+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A44+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A45+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A46+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A47+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A48+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A49+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A50+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A51+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A52+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A53+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A54+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A55+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A56+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A57+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A58+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A59+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A60+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A61+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A62+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A63+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A64+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A65+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A66+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A67+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A68+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A69+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A70+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A71+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A72+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A73+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A74+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A75+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A76+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A77+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A78+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A79+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A80+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A81+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A82+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A83+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A84+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A85+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A86+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A87+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A88+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A89+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A90+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A91+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A92+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A93+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A94+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A95+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A96+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A97+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A98+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A99+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A100+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A101+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A102+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A103+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A104+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A105+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A106+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A107+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A108+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A109+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A110+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A111+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A112+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A113+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A114+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A115+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A116+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A117+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A118+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A119+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A120+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A121+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A122+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A123+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A124+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A125+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A126+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A127+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A128+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A129+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A130+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A131+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A132+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A133+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A134+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A135+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A136+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A137+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A138+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A139+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A140+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A141+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A142+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A143+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A144+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A145+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A146+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A147+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A148+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A149+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A150+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A151+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A152+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A153+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A154+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A155+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A156+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A157+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A158+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" t="str">
+        <f>IF(Table5[[#This Row],[ID_Corrida]] = "", "",A159+1)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -773,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32FBE0-3956-45F0-9B00-3537E8F21FB5}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +1728,7 @@
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
@@ -797,10 +1741,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -813,7 +1757,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -851,7 +1795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -872,7 +1816,7 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GHL-C-S</v>
       </c>
       <c r="I3" s="2"/>
@@ -880,7 +1824,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -901,7 +1845,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GHL-I-S</v>
       </c>
       <c r="I4" s="2"/>
@@ -909,7 +1853,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -930,7 +1874,7 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GH-C-S</v>
       </c>
       <c r="I5" s="2"/>
@@ -938,7 +1882,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -959,7 +1903,7 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GH-I-S</v>
       </c>
       <c r="I6" s="2"/>
@@ -988,7 +1932,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-C-S</v>
       </c>
       <c r="I7" s="2"/>
@@ -1017,7 +1961,7 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-I-S</v>
       </c>
       <c r="I8" s="2"/>
@@ -1046,7 +1990,7 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GLG-C-S</v>
       </c>
       <c r="I9" s="2"/>
@@ -1075,7 +2019,7 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GLG-I-S</v>
       </c>
       <c r="I10" s="2"/>
@@ -1104,7 +2048,7 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-C-S</v>
       </c>
       <c r="I11" s="2"/>
@@ -1133,7 +2077,7 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-I-S</v>
       </c>
       <c r="I12" s="2"/>
@@ -1141,7 +2085,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1149,21 +2093,21 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-C-S</v>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
+        <v>BE-PG-C-S</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1178,7 +2122,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -1187,12 +2131,12 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-I1-S</v>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
+        <v>BE-PG-I1-S</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1207,113 +2151,26 @@
         <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-I2-S</v>
+        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
+        <v>BE-PG-I2-S</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-C-S</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I1-S</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="str">
-        <f>_xlfn.CONCAT(Table14[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I2-S</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1328,10 +2185,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5D3A1B-8CC9-40CC-BB08-44B34DB7A726}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,20 +2509,20 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-C-S</v>
+        <v>BE-PG-C-S</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1676,7 +2533,7 @@
         <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -1685,11 +2542,11 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H14" s="2" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-I1-S</v>
+        <v>BE-PG-I1-S</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1700,90 +2557,18 @@
         <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-DG-I2-S</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="2" t="str">
-        <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-C-S</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="2" t="str">
-        <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I1-S</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H18" s="2" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
         <v>BE-PG-I2-S</v>
       </c>

</xml_diff>

<commit_message>
Put Graph y Bitacora1
</commit_message>
<xml_diff>
--- a/DATABASE/Bitácora.xlsx
+++ b/DATABASE/Bitácora.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Documents\Escuela\6to Sem\Desarrollo de Software\Repositorios\TC3005B-E1\DATABASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD149DF0-5AF6-40F8-A9C6-57FBAB1EFAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0F4095-4561-4F23-A006-4EBD721EB378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AAF969ED-661E-4501-97C9-3B4CFFD775BB}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AAF969ED-661E-4501-97C9-3B4CFFD775BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bitácora" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -159,18 +159,12 @@
     <t>BE-PG-C</t>
   </si>
   <si>
-    <t>El graphID no existe</t>
-  </si>
-  <si>
     <t>El historyID y graphID existen</t>
   </si>
   <si>
     <t>BE-PG-I1</t>
   </si>
   <si>
-    <t>BE-PG-I2</t>
-  </si>
-  <si>
     <t>Actualizar la lista de gráficas</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>ID_Template</t>
   </si>
   <si>
-    <t>BE-PG-I2-E</t>
-  </si>
-  <si>
     <t>BE-PG-I1-E</t>
   </si>
   <si>
@@ -201,7 +192,219 @@
     <t>TM-BE-1</t>
   </si>
   <si>
-    <t>27/05/22</t>
+    <t>{
+  "message": "found",
+  "result": [
+    {
+      "base_file_name": "Analisis_Chatarra_Ene21-ene22",
+      "versions": [
+        {
+          "_id": "Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13",
+          "date": "2022-05-23_18-48-13"
+        }
+      ]
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>114ms</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13</t>
+  </si>
+  <si>
+    <t>{
+  "message": "found",
+  "result": {
+    "historyID": "Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13",
+    "base_file_name": "Analisis_Chatarra_Ene21-ene22",
+    "date": "2022-05-23_18-48-13",
+    "internal_attributes": [
+      "ID_TRANSPORTISTA",
+      "weightDifference",
+      "D_UBICACION",
+      "USUARIO_EGRESO",
+      "N_PESO_TARA",
+      "mediana"
+    ],
+    "external_attributes": [
+      "C_ID_ORDEN_CABECERA",
+      "C_POSICION_ORDEN",
+      "Q_CANTIDAD",
+      "N_PESO_BRUTO",
+      "TIPO_TRANSPORTE"
+    ],
+    "informational_attributes": [
+      "C_SOCIEDAD",
+      "D_PATENTE"
+    ],
+    "graphs": []
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  "message": "Not found"
+}</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-1</t>
+  </si>
+  <si>
+    <t>4ms</t>
+  </si>
+  <si>
+    <t>{
+  "type": "Bar",
+  "labels": [
+    "Largos Puebla",
+    "Gue. Privada Famosa",
+    "L. Apo. Av. Acero",
+    "L. Apo. Av. Camino Mezquital",
+    "Gue. Av. República Mexicana"
+  ],
+  "anomalyList": [
+    8606,
+    4853,
+    2779,
+    9,
+    4
+  ],
+  "noAnomalyList": [
+    837,
+    17028,
+    12082,
+    22,
+    12
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13, D_UBICACION, 0</t>
+  </si>
+  <si>
+    <t>294ms</t>
+  </si>
+  <si>
+    <t>3ms</t>
+  </si>
+  <si>
+    <t>{
+  "type": "Line",
+  "labels": [
+    "Largos Puebla",
+    "Gue. Privada Famosa",
+    "L. Apo. Av. Acero",
+    "Gue. Av. República Mexicana",
+    "L. Apo. Av. Camino Mezquital"
+  ],
+  "anomalyList": [
+    4485,
+    1244,
+    258,
+    1,
+    1
+  ],
+  "noAnomalyList": [
+    4958,
+    20637,
+    14603,
+    15,
+    30
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13, D_UBICACION, -0.05</t>
+  </si>
+  <si>
+    <t>36ms</t>
+  </si>
+  <si>
+    <t>{
+  "type": "Bubble",
+  "data": [
+    {
+      "x": 0,
+      "y": 0,
+      "r": 25
+    },
+    ...
+  ],
+  "attribute1Dict": [
+    "Largos Puebla",
+    "Gue. Privada Famosa",
+    "L. Apo. Av. Acero",
+    "Gue. Av. República Mexicana",
+    "L. Apo. Av. Camino Mezquital"
+  ],
+  "attribute2Dict": [
+    "Full Neumática",
+    "Torton",
+    "Contenedor Sobre Plataforma",
+    "CONTENEDOR CHATARRA",
+    "TOLVA",
+    "Plataforma 3 ejes Neumática",
+    "Camioneta 3.5",
+    "Plataforma 2 ejes Neumática",
+    "Unidad Tractora",
+    "SEMIREMOLQUE",
+    "Plataforma 2 ejes Muelles",
+    "Plataforma 3 ejes Muelles",
+    "NA"
+  ]
+}</t>
+  </si>
+  <si>
+    <t>138ms</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-13, D_UBICACION, TIPO_TRANSPORTE, -0.05</t>
+  </si>
+  <si>
+    <t>24ms</t>
+  </si>
+  <si>
+    <t>5ms</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-1, D_UBICACION, TIPO_TRANSPORTE, -0.05</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-1, D_UBICACION, -0.05</t>
+  </si>
+  <si>
+    <t>Analisis_Chatarra_Ene21-ene22_2022-05-23_18-48-1, D_UBICACION, 0</t>
+  </si>
+  <si>
+    <t>BE-PG-I-E</t>
+  </si>
+  <si>
+    <t>BE-PG-I</t>
+  </si>
+  <si>
+    <t>{
+  "message": "Success"
+}</t>
+  </si>
+  <si>
+    <t>7ms</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ignorada</t>
+  </si>
+  <si>
+    <t>No se realizó la BE-GHL-I por falta de una segunda BD</t>
+  </si>
+  <si>
+    <t>27/05/22 (11:15)</t>
   </si>
 </sst>
 </file>
@@ -237,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,13 +454,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -266,7 +479,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -369,44 +582,44 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}" name="Table13" displayName="Table13" ref="A2:L15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A2:L15" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}" name="Table13" displayName="Table13" ref="A2:L14" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:L14" xr:uid="{F654FED4-1A8D-476E-A37C-BEE1A454A39E}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{7B09FA86-D36E-427E-97CF-B7D8B36AB84D}" name="Sec" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{39FB757B-3C82-4EE3-B429-5F23FAE004D8}" name="ID" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E942E4FC-8D92-4234-B6B1-D6F263244207}" name="Descripción" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{D732C358-F448-4B04-BBD0-ECFC5897E549}" name="Caso / Precondición" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{88CFCC99-ADBC-4B05-BF00-0D841EBA5F1A}" name="Tipo" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{BAB65155-53CC-4710-9605-1A048D68DF00}" name="Entrada Esperada" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{241B06ED-06A5-4504-9EC6-16FA523F3ED5}" name="Entrada Dada" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2187D5F3-18A4-48C5-9F3F-BAA1BFEE46C7}" name="Salida Esperada" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{7B09FA86-D36E-427E-97CF-B7D8B36AB84D}" name="Sec" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{39FB757B-3C82-4EE3-B429-5F23FAE004D8}" name="ID" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{E942E4FC-8D92-4234-B6B1-D6F263244207}" name="Descripción" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{D732C358-F448-4B04-BBD0-ECFC5897E549}" name="Caso / Precondición" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{88CFCC99-ADBC-4B05-BF00-0D841EBA5F1A}" name="Tipo" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{BAB65155-53CC-4710-9605-1A048D68DF00}" name="Entrada Esperada" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{241B06ED-06A5-4504-9EC6-16FA523F3ED5}" name="Entrada Dada" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{2187D5F3-18A4-48C5-9F3F-BAA1BFEE46C7}" name="Salida Esperada" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{5C7873B5-E430-4D40-B78D-AE61CA6C7E13}" name="Salida Dada" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{0A23A4F0-5E33-44D3-9E82-A08C36D88BB2}" name="Tiempo" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{D8C2EF58-1D1F-4BD9-8949-5D5B023DF187}" name="Comentarios" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{2601F79F-09FF-427D-844A-A77E3E54B807}" name="Estatus" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{5C7873B5-E430-4D40-B78D-AE61CA6C7E13}" name="Salida Dada" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{0A23A4F0-5E33-44D3-9E82-A08C36D88BB2}" name="Tiempo" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{D8C2EF58-1D1F-4BD9-8949-5D5B023DF187}" name="Comentarios" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{2601F79F-09FF-427D-844A-A77E3E54B807}" name="Estatus" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L15" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A2:L15" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}" name="Table1" displayName="Table1" ref="A2:L14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A2:L14" xr:uid="{D625F29E-6A25-4577-8594-0B5DF729A98A}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{B7680AA0-D54F-49B5-A63F-1F891CC4C50F}" name="Sec" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{A22F15E3-092B-4136-A538-B8FA3464ABF0}" name="ID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{2C4195F3-597B-470F-8A24-6CD709DE2A42}" name="Descripción" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{BCCFA00E-82C7-4FBA-838B-5CFD93D14B7B}" name="Caso / Precondición" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{58C386C7-020E-4EB6-A4FF-630F8D8BC905}" name="Tipo" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{BE11E4E5-9984-4F3A-A79D-2F3C01C30543}" name="Entrada Esperada" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{11AA7622-AC33-4821-BF0A-5364407BDCC5}" name="Entrada Dada" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{916248A3-AD1D-48E7-AE3E-95114FE8C1A2}" name="Salida Esperada" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{2D2E824C-86C2-48A1-A914-33DC99D04576}" name="Salida Dada" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{20E86714-D65A-498F-9CB8-6D8DA81F52A3}" name="Tiempo" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{59411D5E-44C5-4B3E-9510-1EE82744BA36}" name="Comentarios" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{BB23AAD6-DCFE-433A-A880-3ABBBB8CBEEE}" name="Estatus" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32710F9C-3D4D-4EFE-8BF9-3040E30C63EB}">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,16 +940,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
-        <v>47</v>
-      </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
         <v>7</v>
@@ -750,13 +963,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1717,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32FBE0-3956-45F0-9B00-3537E8F21FB5}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,9 +1950,9 @@
     <col min="4" max="4" width="30.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="6" customWidth="1"/>
     <col min="8" max="8" width="14.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="6" customWidth="1"/>
     <col min="10" max="10" width="10" style="1" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="1"/>
@@ -1741,10 +1960,10 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1776,13 +1995,13 @@
       <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -1814,15 +2033,23 @@
       <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="H3" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GHL-C-S</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="I3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -1843,15 +2070,25 @@
       <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="H4" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GHL-I-S</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="I4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -1872,15 +2109,23 @@
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="H5" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GH-C-S</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -1901,15 +2146,23 @@
       <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="H6" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GH-I-S</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="I6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -1930,15 +2183,23 @@
       <c r="F7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="H7" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-C-S</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -1959,15 +2220,23 @@
       <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="H8" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-I-S</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
@@ -1988,15 +2257,23 @@
       <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="H9" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GLG-C-S</v>
       </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="L9" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -2017,15 +2294,23 @@
       <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="H10" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GLG-I-S</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -2046,15 +2331,23 @@
       <c r="F11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="H11" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-C-S</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="I11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="L11" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
@@ -2075,15 +2368,23 @@
       <c r="F12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="H12" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-GBG-I-S</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
+      <c r="L12" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
@@ -2093,36 +2394,44 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="H13" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-PG-C-S</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="I13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -2131,46 +2440,25 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>57</v>
+      </c>
       <c r="H14" s="2" t="str">
         <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
         <v>BE-PG-I1-S</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="str">
-        <f>_xlfn.CONCAT(Table13[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I2-S</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="L14" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2185,10 +2473,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5D3A1B-8CC9-40CC-BB08-44B34DB7A726}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2209,7 +2497,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -2509,16 +2797,16 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
@@ -2530,10 +2818,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>29</v>
@@ -2542,35 +2830,11 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="H14" s="2" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I1-S</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="2" t="str">
-        <f>_xlfn.CONCAT(Table1[[#This Row],[ID]], "-S")</f>
-        <v>BE-PG-I2-S</v>
+        <v>BE-PG-I-S</v>
       </c>
     </row>
   </sheetData>

</xml_diff>